<commit_message>
Fixed form to use /data root node (#21)
</commit_message>
<xml_diff>
--- a/docs/counter.xlsx
+++ b/docs/counter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">increment=true()</t>
   </si>
   <si>
-    <t xml:space="preserve">ex:org.opendatakit.counter(form_id='counter-form', form_name=jr:itext('/counter/form_name:label'), question_id='2', question_name=jr:itext('/counter/counter2:label'), increment=true())</t>
+    <t xml:space="preserve">ex:org.opendatakit.counter(form_id='counter-form', form_name=jr:itext('/data/form_name:label'), question_id='2', question_name=jr:itext('/data/counter2:label'), increment=true())</t>
   </si>
   <si>
     <t xml:space="preserve">note</t>
@@ -276,19 +276,19 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="202.719387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="14.1734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="202.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -372,7 +372,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>